<commit_message>
Updated the scripts for demo
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>password</t>
   </si>
@@ -40,6 +40,15 @@
   </si>
   <si>
     <t>1!Qa1!Qa</t>
+  </si>
+  <si>
+    <t>MummsAdmin</t>
+  </si>
+  <si>
+    <t>j.pandala@mumms.com</t>
+  </si>
+  <si>
+    <t>J@iram18</t>
   </si>
 </sst>
 </file>
@@ -433,7 +442,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -463,70 +472,70 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="F4" s="6"/>
+      <c r="B4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="3"/>
+      <c r="D5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
+      <c r="D6" s="6"/>
+      <c r="F6" s="6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
-      <c r="C7" s="3"/>
       <c r="D7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="D8" s="6"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="F10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-    <hyperlink ref="C2" r:id="rId2" display="J@iram18"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2" display="J@iram18"/>
+    <hyperlink ref="B2" r:id="rId3"/>
+    <hyperlink ref="C2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated framework. New methods have been added
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\MummsFrameWork\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="420" windowWidth="14295" windowHeight="4320"/>
+    <workbookView xWindow="480" yWindow="600" windowWidth="14295" windowHeight="4140"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>password</t>
   </si>
@@ -30,25 +25,28 @@
     <t>username</t>
   </si>
   <si>
-    <t xml:space="preserve">HospicesUser </t>
+    <t>HospiceUser</t>
   </si>
   <si>
     <t>1!Qa1!Qa</t>
   </si>
   <si>
-    <t>MummsAdmin</t>
-  </si>
-  <si>
-    <t>j.pandala@mumms.com</t>
-  </si>
-  <si>
-    <t>J@iram18</t>
+    <t>a.muchakhandi@mumms.com</t>
+  </si>
+  <si>
+    <t>AdminUser 1</t>
+  </si>
+  <si>
+    <t>p.chidri@mumms.com</t>
+  </si>
+  <si>
+    <t>Cigniti@123</t>
+  </si>
+  <si>
+    <t>a.muchakhandi-anilgallop@mumms.com</t>
   </si>
   <si>
     <t>AdminUser</t>
-  </si>
-  <si>
-    <t>a.muchakhandi-testorl@mumms.com</t>
   </si>
 </sst>
 </file>
@@ -148,9 +146,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -198,7 +193,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -233,7 +228,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -442,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,41 +467,45 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="6"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3"/>
+        <v>10</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="6"/>
-      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
+      <c r="C6" s="3"/>
       <c r="D6" s="6"/>
       <c r="F6" s="6"/>
     </row>
@@ -515,27 +514,33 @@
       <c r="D7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="D8" s="6"/>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4"/>
       <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2" display="J@iram18"/>
-    <hyperlink ref="B2" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2" display="Cigniti@123"/>
+    <hyperlink ref="B3" r:id="rId3"/>
+    <hyperlink ref="B4" r:id="rId4"/>
+    <hyperlink ref="C4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
04062016 - Latest Code commited to the git
</commit_message>
<xml_diff>
--- a/TestData/LoginData.xlsx
+++ b/TestData/LoginData.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\172.16.2.5\CShare\Gallop\Idexx\Praveen\MummsFrameWork-04052016\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="600" windowWidth="14295" windowHeight="4140"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="9" r:id="rId1"/>
@@ -25,16 +30,13 @@
     <t>username</t>
   </si>
   <si>
-    <t>HospiceUser</t>
-  </si>
-  <si>
     <t>1!Qa1!Qa</t>
   </si>
   <si>
     <t>a.muchakhandi@mumms.com</t>
   </si>
   <si>
-    <t>AdminUser 1</t>
+    <t>AdminUser</t>
   </si>
   <si>
     <t>p.chidri@mumms.com</t>
@@ -43,10 +45,13 @@
     <t>Cigniti@123</t>
   </si>
   <si>
-    <t>a.muchakhandi-anilgallop@mumms.com</t>
-  </si>
-  <si>
-    <t>AdminUser</t>
+    <t>AdminUser1</t>
+  </si>
+  <si>
+    <t>ReportsUser</t>
+  </si>
+  <si>
+    <t>a.muchakhandi-testbronx@mumms.com</t>
   </si>
 </sst>
 </file>
@@ -146,6 +151,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -193,7 +201,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,7 +236,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -437,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,78 +475,69 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="5"/>
-      <c r="C5" s="3"/>
+      <c r="D5" s="6"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5"/>
-      <c r="C6" s="3"/>
       <c r="D6" s="6"/>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
       <c r="B7" s="5"/>
       <c r="D7" s="6"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="F8" s="6"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B9" s="5"/>
-      <c r="D9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="C2" r:id="rId2" display="Cigniti@123"/>
     <hyperlink ref="B3" r:id="rId3"/>
-    <hyperlink ref="B4" r:id="rId4"/>
-    <hyperlink ref="C4" r:id="rId5"/>
+    <hyperlink ref="C3" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId6"/>

</xml_diff>